<commit_message>
adding api lib working copy
</commit_message>
<xml_diff>
--- a/src/example/datafile/APIDataFile.xlsx
+++ b/src/example/datafile/APIDataFile.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -10,12 +10,12 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="FP Flow" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Endpoint</t>
   </si>
@@ -110,12 +110,15 @@
     <t>data.commodities[0].color
 data.commodities[0].name</t>
   </si>
+  <si>
+    <t>ExpectedStatuscode</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,7 +288,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -320,7 +322,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -496,25 +497,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="33.42578125" customWidth="1"/>
     <col min="3" max="3" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="75.28515625" customWidth="1"/>
-    <col min="8" max="8" width="69.85546875" customWidth="1"/>
+    <col min="5" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="75.28515625" customWidth="1"/>
+    <col min="9" max="9" width="69.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -531,13 +532,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="42.75" customHeight="1" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -556,10 +560,13 @@
       <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2">
+        <v>200</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -573,14 +580,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="39.42578125" customWidth="1"/>
@@ -592,7 +599,7 @@
     <col min="8" max="8" width="45.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="4" customFormat="1">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -615,7 +622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="75">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -637,7 +644,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="86.25" customHeight="1">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -663,7 +670,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -686,13 +693,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="B5" s="1"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:8" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15.75" thickBot="1"/>
+    <row r="9" spans="1:8" ht="42.75" customHeight="1" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>

</xml_diff>